<commit_message>
sorting goal minute 0
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/eu/best_four_third_teams_eu_uefa.xlsx
+++ b/data/out/wiki/men/uefa/eu/best_four_third_teams_eu_uefa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,11 @@
           <t>Group F</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>half_time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -588,6 +593,7 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -662,6 +668,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -736,6 +745,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -810,6 +822,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -884,6 +899,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -958,6 +976,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1032,6 +1053,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1106,6 +1130,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1180,6 +1207,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1254,6 +1284,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1328,6 +1361,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1402,6 +1438,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1476,6 +1515,9 @@
           <t>['Portugal', 3, 0, 1]</t>
         </is>
       </c>
+      <c r="Q14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1550,6 +1592,9 @@
           <t>['Portugal', 2, -1, 1]</t>
         </is>
       </c>
+      <c r="Q15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1624,6 +1669,9 @@
           <t>['Portugal', 3, 0, 2]</t>
         </is>
       </c>
+      <c r="Q16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1698,6 +1746,9 @@
           <t>['Portugal', 2, -1, 2]</t>
         </is>
       </c>
+      <c r="Q17" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1772,6 +1823,9 @@
           <t>['Portugal', 3, 0, 3]</t>
         </is>
       </c>
+      <c r="Q18" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1846,6 +1900,9 @@
           <t>['Portugal', 2, -1, 3]</t>
         </is>
       </c>
+      <c r="Q19" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1920,6 +1977,9 @@
           <t>['Portugal', 2, -1, 3]</t>
         </is>
       </c>
+      <c r="Q20" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1994,6 +2054,9 @@
           <t>['Iceland', 3, 0, 3]</t>
         </is>
       </c>
+      <c r="Q21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2068,6 +2131,9 @@
           <t>['Portugal', 3, 0, 4]</t>
         </is>
       </c>
+      <c r="Q22" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2142,6 +2208,9 @@
           <t>['Portugal', 3, 0, 4]</t>
         </is>
       </c>
+      <c r="Q23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2216,13 +2285,16 @@
           <t>['Portugal', 3, 0, 4]</t>
         </is>
       </c>
+      <c r="Q24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>2021</v>
       </c>
       <c r="B25" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2241,12 +2313,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Spain']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Croatia', 'Switzerland']</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2262,7 +2334,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>['Switzerland', 4, -2, 2]</t>
+          <t>['Switzerland', 2, -3, 1]</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2272,7 +2344,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2290,13 +2362,14 @@
           <t>['Portugal', 4, 1, 5]</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>2021</v>
       </c>
       <c r="B26" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -2315,12 +2388,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Switzerland']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2329,14 +2402,14 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>['Switzerland', 4, -1, 3]</t>
+          <t>['Switzerland', 4, -2, 2]</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2346,7 +2419,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2363,6 +2436,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -2370,7 +2446,7 @@
         <v>2021</v>
       </c>
       <c r="B27" t="n">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -2389,12 +2465,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Switzerland']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2406,11 +2482,11 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>['Switzerland', 4, -2, 3]</t>
+          <t>['Switzerland', 4, -1, 3]</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2420,7 +2496,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2437,6 +2513,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2444,7 +2523,7 @@
         <v>2021</v>
       </c>
       <c r="B28" t="n">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -2463,12 +2542,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Switzerland']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2480,11 +2559,11 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>['Switzerland', 4, -1, 4]</t>
+          <t>['Switzerland', 4, -2, 3]</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2494,7 +2573,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2511,6 +2590,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -2518,7 +2600,7 @@
         <v>2021</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -2527,7 +2609,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2537,12 +2619,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Switzerland']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2554,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2568,7 +2650,7 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -2585,6 +2667,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -2611,12 +2696,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['Finland', 'Portugal', 'Spain', 'Switzerland']</t>
+          <t>['Austria', 'Finland', 'Portugal', 'Switzerland']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Croatia']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2628,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -2642,7 +2727,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>['Ukraine', 3, -1, 4]</t>
+          <t>['Austria', 4, 0, 3]</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2659,6 +2744,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -2699,10 +2787,10 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -2733,6 +2821,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -2776,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -2807,6 +2898,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -2850,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -2881,6 +2975,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -2924,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2955,6 +3052,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -2998,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -3029,6 +3129,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -3072,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -3103,6 +3206,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q36" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -3146,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -3177,6 +3283,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -3220,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -3251,6 +3360,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q38" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -3294,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -3325,6 +3437,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -3368,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -3399,6 +3514,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -3442,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
@@ -3473,6 +3591,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q41" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -3516,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -3547,6 +3668,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -3590,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -3621,6 +3745,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q43" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -3664,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="J44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -3695,6 +3822,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -3738,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -3769,6 +3899,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -3812,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -3843,6 +3976,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -3886,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -3917,6 +4053,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -3960,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -3991,6 +4130,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q48" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -4034,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4065,6 +4207,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q49" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -4108,7 +4253,7 @@
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -4139,6 +4284,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -4182,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -4213,6 +4361,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q51" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -4256,7 +4407,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -4287,6 +4438,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q52" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -4330,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -4361,6 +4515,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q53" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -4404,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -4435,6 +4592,9 @@
         <is>
           <t>['Portugal', 4, 1, 5]</t>
         </is>
+      </c>
+      <c r="Q54" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -4478,7 +4638,7 @@
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -4509,6 +4669,9 @@
         <is>
           <t>['Hungary', 4, -2, 2]</t>
         </is>
+      </c>
+      <c r="Q55" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -4552,7 +4715,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -4583,6 +4746,9 @@
         <is>
           <t>['Hungary', 4, -2, 2]</t>
         </is>
+      </c>
+      <c r="Q56" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -4626,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -4657,6 +4823,9 @@
         <is>
           <t>['Germany', 3, 0, 4]</t>
         </is>
+      </c>
+      <c r="Q57" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -4700,7 +4869,7 @@
         <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -4731,6 +4900,9 @@
         <is>
           <t>['Hungary', 4, -2, 2]</t>
         </is>
+      </c>
+      <c r="Q58" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -4774,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -4805,6 +4977,9 @@
         <is>
           <t>['Portugal', 4, 1, 7]</t>
         </is>
+      </c>
+      <c r="Q59" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -4831,7 +5006,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>['Albania', 'Austria', 'Denmark', 'Slovakia']</t>
+          <t>['Albania', 'Austria', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -4872,7 +5047,7 @@
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4880,6 +5055,7 @@
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
       </c>
+      <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4905,7 +5081,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['Albania', 'Austria', 'Denmark', 'Slovakia']</t>
+          <t>['Albania', 'Austria', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -4946,13 +5122,16 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q61" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -4979,7 +5158,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>['Albania', 'Austria', 'Denmark', 'Slovakia']</t>
+          <t>['Albania', 'Austria', 'Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -5020,13 +5199,16 @@
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q62" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -5053,7 +5235,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -5094,13 +5276,16 @@
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q63" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -5127,7 +5312,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -5168,13 +5353,16 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q64" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -5201,7 +5389,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Italy', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Italy']</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -5242,13 +5430,16 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q65" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -5275,7 +5466,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -5316,13 +5507,16 @@
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q66" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -5349,7 +5543,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>['Denmark', 'Hungary', 'Netherlands', 'Slovakia']</t>
+          <t>['Belgium', 'Denmark', 'Hungary', 'Netherlands']</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -5359,7 +5553,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Slovakia']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5390,13 +5584,16 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q67" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -5423,7 +5620,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -5464,13 +5661,16 @@
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q68" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -5497,7 +5697,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -5538,13 +5738,16 @@
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -5571,7 +5774,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>['Denmark', 'Hungary', 'Netherlands', 'Slovakia']</t>
+          <t>['Belgium', 'Denmark', 'Hungary', 'Netherlands']</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -5612,13 +5815,16 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q70" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -5645,7 +5851,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -5686,13 +5892,16 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q71" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -5719,7 +5928,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>['Austria', 'Denmark', 'Hungary', 'Slovakia']</t>
+          <t>['Austria', 'Belgium', 'Denmark', 'Hungary']</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -5760,13 +5969,16 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q72" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -5793,7 +6005,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>['Denmark', 'Hungary', 'Netherlands', 'Slovakia']</t>
+          <t>['Belgium', 'Denmark', 'Hungary', 'Netherlands']</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -5834,13 +6046,16 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 2]</t>
+          <t>['Belgium', 4, 1, 2]</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
+      </c>
+      <c r="Q73" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -5916,6 +6131,9 @@
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
       </c>
+      <c r="Q74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5990,6 +6208,9 @@
           <t>['Czech Republic', 2, -1, 2]</t>
         </is>
       </c>
+      <c r="Q75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -6064,6 +6285,9 @@
           <t>['Georgia', 4, -1, 3]</t>
         </is>
       </c>
+      <c r="Q76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -6138,6 +6362,9 @@
           <t>['Georgia', 4, -1, 3]</t>
         </is>
       </c>
+      <c r="Q77" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -6212,6 +6439,9 @@
           <t>['Georgia', 4, 0, 4]</t>
         </is>
       </c>
+      <c r="Q78" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -6286,6 +6516,9 @@
           <t>['Georgia', 4, 0, 4]</t>
         </is>
       </c>
+      <c r="Q79" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -6359,6 +6592,9 @@
         <is>
           <t>['Georgia', 4, 0, 4]</t>
         </is>
+      </c>
+      <c r="Q80" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>